<commit_message>
DPLK 1 - 10, 67 - 71, 76(Belom Kelar)
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKKLM001-007 - Setup Jenis Dokumen Klaim - Setup Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKKLM001-007 - Setup Jenis Dokumen Klaim - Setup Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DPLK 2\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2427B1C7-072C-4604-92DC-180EBFA5BB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3460158-05F9-4665-B9A8-E7DEC64E63CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="35">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -61,9 +61,6 @@
     <t>MAIN_SIDEBAR</t>
   </si>
   <si>
-    <t>Setup</t>
-  </si>
-  <si>
     <t>Tambah Data Dapat dilakukan dengan baik</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
   </si>
   <si>
     <t>Klaim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Setup Jenis Dokumen </t>
   </si>
   <si>
     <t>DPLKKLM001-007</t>
@@ -129,6 +123,15 @@
     <t>Username : Putri,
 Password : bni1234/,
 Kode Jenis Dokumen    : 11223</t>
+  </si>
+  <si>
+    <t>Setup Jenis Dokumen,0</t>
+  </si>
+  <si>
+    <t>Setup Jenis Dokumen ,0</t>
+  </si>
+  <si>
+    <t>Setup,0</t>
   </si>
 </sst>
 </file>
@@ -530,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F4:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>8</v>
@@ -596,10 +599,10 @@
         <v>2</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -615,19 +618,19 @@
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>10</v>
@@ -636,20 +639,20 @@
         <v>11</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="5">
         <v>11223</v>
       </c>
       <c r="N2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O2" s="5"/>
       <c r="P2" s="7"/>
@@ -665,19 +668,19 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>23</v>
-      </c>
       <c r="E3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>10</v>
@@ -686,20 +689,20 @@
         <v>11</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="5">
         <v>11223</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="O3" s="5"/>
       <c r="P3" s="7"/>
@@ -715,19 +718,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>10</v>
@@ -736,13 +739,13 @@
         <v>11</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="5">
@@ -763,19 +766,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>10</v>
@@ -784,13 +787,13 @@
         <v>11</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="5">

</xml_diff>